<commit_message>
Modified 05/08/2024 03:22:33 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
@@ -153,19 +153,119 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>20</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>25</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>20</col>
+      <colOff>0</colOff>
+      <row>20</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -180,107 +280,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>50</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>75</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>100</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>125</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>150</row>
+      <row>40</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -303,9 +303,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>175</row>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>40</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -328,9 +328,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>200</row>
+      <col>20</col>
+      <colOff>0</colOff>
+      <row>40</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -643,14 +643,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1"/>
+    <row r="21"/>
+    <row r="41"/>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified 05/08/2024 03:26:19 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
@@ -205,7 +205,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>20</row>
+      <row>30</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -230,7 +230,7 @@
     <from>
       <col>10</col>
       <colOff>0</colOff>
-      <row>20</row>
+      <row>30</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -255,7 +255,7 @@
     <from>
       <col>20</col>
       <colOff>0</colOff>
-      <row>20</row>
+      <row>30</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -280,7 +280,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>40</row>
+      <row>60</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -305,7 +305,7 @@
     <from>
       <col>10</col>
       <colOff>0</colOff>
-      <row>40</row>
+      <row>60</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -330,7 +330,7 @@
     <from>
       <col>20</col>
       <colOff>0</colOff>
-      <row>40</row>
+      <row>60</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -643,7 +643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -652,8 +652,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1"/>
-    <row r="21"/>
-    <row r="41"/>
+    <row r="31"/>
+    <row r="61"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Modified 05/08/2024 03:28:19 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise graphs/2020_cars_combined.xlsx
@@ -178,9 +178,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>20</col>
-      <colOff>0</colOff>
-      <row>0</row>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>30</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -203,19 +203,44 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>30</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>30</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+      <row>60</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -230,32 +255,7 @@
     <from>
       <col>10</col>
       <colOff>0</colOff>
-      <row>30</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6000750" cy="4476750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>20</col>
-      <colOff>0</colOff>
-      <row>30</row>
+      <row>60</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -280,7 +280,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>60</row>
+      <row>90</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -305,7 +305,7 @@
     <from>
       <col>10</col>
       <colOff>0</colOff>
-      <row>60</row>
+      <row>90</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -328,9 +328,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>20</col>
-      <colOff>0</colOff>
-      <row>60</row>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>120</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="6000750" cy="4476750"/>
@@ -643,7 +643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,6 +654,8 @@
     <row r="1"/>
     <row r="31"/>
     <row r="61"/>
+    <row r="91"/>
+    <row r="121"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>